<commit_message>
Implemented Cantera emission calculation, emission plot script and bug fixes
</commit_message>
<xml_diff>
--- a/input_data/LV_Database.xlsx
+++ b/input_data/LV_Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan-Steffen Fischer\Desktop\test_cea\glen_cea\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan-Steffen Fischer\Desktop\LEAT_to_update\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9547F6B7-8B59-44CB-A1C0-D41823E19EA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBC4879-0C0C-4446-90F1-50B2EF8EFC61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LV_Database" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="155">
   <si>
     <t>sheet: LV_Database</t>
   </si>
@@ -472,6 +472,24 @@
   </si>
   <si>
     <t>Reference cross sectional area</t>
+  </si>
+  <si>
+    <t>H2_Test</t>
+  </si>
+  <si>
+    <t>CH4_Test</t>
+  </si>
+  <si>
+    <t>CH4(L)/O2(L)</t>
+  </si>
+  <si>
+    <t>110/90</t>
+  </si>
+  <si>
+    <t>20/90</t>
+  </si>
+  <si>
+    <t>d_exit</t>
   </si>
 </sst>
 </file>
@@ -581,7 +599,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -937,12 +955,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1153,54 +1184,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1504,10 +1497,10 @@
   <dimension ref="A1:BU12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2249,7 +2242,7 @@
         <v>5.2</v>
       </c>
       <c r="G5" s="42">
-        <f t="shared" ref="G5:G6" si="4">PI()/4*F5^2</f>
+        <f t="shared" ref="G5:G8" si="4">PI()/4*F5^2</f>
         <v>21.237166338267002</v>
       </c>
       <c r="H5" s="48" t="s">
@@ -2557,7 +2550,103 @@
       <c r="BT6" s="64"/>
       <c r="BU6" s="73"/>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:73" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="41">
+        <v>70</v>
+      </c>
+      <c r="C7" s="42">
+        <v>3.7</v>
+      </c>
+      <c r="D7" s="42">
+        <v>2.9</v>
+      </c>
+      <c r="E7" s="42">
+        <v>1.8</v>
+      </c>
+      <c r="F7" s="42">
+        <v>5.2</v>
+      </c>
+      <c r="G7" s="42">
+        <f t="shared" si="4"/>
+        <v>21.237166338267002</v>
+      </c>
+      <c r="H7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="43">
+        <v>7607000</v>
+      </c>
+      <c r="J7" s="43">
+        <v>8227000</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="L7" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="M7" s="45">
+        <v>410900</v>
+      </c>
+      <c r="N7" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="O7" s="45">
+        <f t="shared" ref="O7:O8" si="5">M7*1/(2.36+1)</f>
+        <v>122291.66666666667</v>
+      </c>
+      <c r="P7" s="45">
+        <f t="shared" ref="P7:P8" si="6">M7*2.36/(2.36+1)</f>
+        <v>288608.33333333337</v>
+      </c>
+      <c r="Q7" s="45">
+        <v>22200</v>
+      </c>
+      <c r="R7" s="45">
+        <v>162</v>
+      </c>
+      <c r="S7" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="U7" s="49">
+        <v>981000</v>
+      </c>
+      <c r="V7" s="49">
+        <v>981000</v>
+      </c>
+      <c r="W7" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="X7" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y7" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z7" s="45">
+        <v>107500</v>
+      </c>
+      <c r="AA7" s="45">
+        <f>Z7*1/(2.36+1)</f>
+        <v>31994.047619047622</v>
+      </c>
+      <c r="AB7" s="45">
+        <f>AA7*2.36/(2.36+1)</f>
+        <v>22472.00963718821</v>
+      </c>
+      <c r="AC7" s="45">
+        <f>4000+1700+22800</f>
+        <v>28500</v>
+      </c>
+      <c r="AD7" s="45">
+        <v>397</v>
+      </c>
       <c r="BM7" s="67"/>
       <c r="BN7" s="68"/>
       <c r="BO7" s="69"/>
@@ -2568,7 +2657,103 @@
       <c r="BT7" s="72"/>
       <c r="BU7" s="73"/>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:73" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="41">
+        <v>70</v>
+      </c>
+      <c r="C8" s="42">
+        <v>3.7</v>
+      </c>
+      <c r="D8" s="42">
+        <v>2.9</v>
+      </c>
+      <c r="E8" s="42">
+        <v>1.8</v>
+      </c>
+      <c r="F8" s="42">
+        <v>5.2</v>
+      </c>
+      <c r="G8" s="42">
+        <f t="shared" si="4"/>
+        <v>21.237166338267002</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="43">
+        <v>7607000</v>
+      </c>
+      <c r="J8" s="43">
+        <v>8227000</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="M8" s="45">
+        <v>410900</v>
+      </c>
+      <c r="N8" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="O8" s="45">
+        <f t="shared" si="5"/>
+        <v>122291.66666666667</v>
+      </c>
+      <c r="P8" s="45">
+        <f t="shared" si="6"/>
+        <v>288608.33333333337</v>
+      </c>
+      <c r="Q8" s="45">
+        <v>22200</v>
+      </c>
+      <c r="R8" s="45">
+        <v>162</v>
+      </c>
+      <c r="S8" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="U8" s="49">
+        <v>981000</v>
+      </c>
+      <c r="V8" s="49">
+        <v>981000</v>
+      </c>
+      <c r="W8" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="X8" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y8" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z8" s="45">
+        <v>107500</v>
+      </c>
+      <c r="AA8" s="45">
+        <f>Z8*1/(2.36+1)</f>
+        <v>31994.047619047622</v>
+      </c>
+      <c r="AB8" s="45">
+        <f>AA8*2.36/(2.36+1)</f>
+        <v>22472.00963718821</v>
+      </c>
+      <c r="AC8" s="45">
+        <f>4000+1700+22800</f>
+        <v>28500</v>
+      </c>
+      <c r="AD8" s="45">
+        <v>397</v>
+      </c>
       <c r="AI8" s="54"/>
       <c r="BM8" s="67"/>
       <c r="BN8" s="68"/>
@@ -2634,10 +2819,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2645,10 +2830,11 @@
     <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>51</v>
       </c>
@@ -2658,11 +2844,14 @@
       <c r="C1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="75" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -2672,11 +2861,14 @@
       <c r="C2" s="2">
         <v>115</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2686,11 +2878,14 @@
       <c r="C3" s="28">
         <v>70</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="28">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -2700,11 +2895,14 @@
       <c r="C4" s="2">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2714,11 +2912,14 @@
       <c r="C5" s="2">
         <v>206</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -2728,11 +2929,14 @@
       <c r="C6" s="2">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2742,11 +2946,14 @@
       <c r="C7" s="2">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -2756,11 +2963,14 @@
       <c r="C8" s="2">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -2770,11 +2980,14 @@
       <c r="C9" s="2">
         <v>97</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -2784,11 +2997,14 @@
       <c r="C10" s="2">
         <v>100</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -2798,11 +3014,14 @@
       <c r="C11" s="2">
         <v>100</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2812,11 +3031,14 @@
       <c r="C12" s="2">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -2826,8 +3048,11 @@
       <c r="C13" s="29">
         <v>105</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>132</v>
       </c>
@@ -2837,8 +3062,11 @@
       <c r="C14">
         <v>118.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -2847,6 +3075,9 @@
       </c>
       <c r="C15" s="29">
         <v>60</v>
+      </c>
+      <c r="D15" s="29">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>